<commit_message>
Did VBA for input template
</commit_message>
<xml_diff>
--- a/Postprocessing Notebooks/Results.xlsx
+++ b/Postprocessing Notebooks/Results.xlsx
@@ -343,42 +343,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:E4"/>
+  <dimension ref="C2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:3">
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5">
+    </row>
+    <row r="3" spans="3:3">
       <c r="C3">
         <v>-0</v>
       </c>
-      <c r="D3">
-        <v>-0</v>
-      </c>
-      <c r="E3">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5">
+    </row>
+    <row r="4" spans="3:3">
       <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
         <v>10</v>
       </c>
     </row>
@@ -389,42 +371,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:E4"/>
+  <dimension ref="C2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:3">
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5">
+    </row>
+    <row r="3" spans="3:3">
       <c r="C3">
         <v>-0</v>
       </c>
-      <c r="D3">
-        <v>-0</v>
-      </c>
-      <c r="E3">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5">
+    </row>
+    <row r="4" spans="3:3">
       <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
         <v>10</v>
       </c>
     </row>
@@ -435,42 +399,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:E4"/>
+  <dimension ref="C2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:3">
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5">
+    </row>
+    <row r="3" spans="3:3">
       <c r="C3">
         <v>-0</v>
       </c>
-      <c r="D3">
-        <v>-0</v>
-      </c>
-      <c r="E3">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5">
+    </row>
+    <row r="4" spans="3:3">
       <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
         <v>10</v>
       </c>
     </row>
@@ -481,42 +427,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:E4"/>
+  <dimension ref="C2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:3">
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5">
+    </row>
+    <row r="3" spans="3:3">
       <c r="C3">
         <v>-0</v>
       </c>
-      <c r="D3">
-        <v>-0</v>
-      </c>
-      <c r="E3">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5">
+    </row>
+    <row r="4" spans="3:3">
       <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
         <v>10</v>
       </c>
     </row>

</xml_diff>